<commit_message>
adding four more dataframe
</commit_message>
<xml_diff>
--- a/output/summary_mean_totals.xlsx
+++ b/output/summary_mean_totals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amerifleet-my.sharepoint.com/personal/jared_saeger_acertusdelivers_com/Documents/Desktop/BootCamp/Homework/07-project_one/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D1AA2438-2A43-4666-9823-FA2039F2AE1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AA85F0B3-2A69-4068-9345-9F063E346F59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="5295" yWindow="2595" windowWidth="28770" windowHeight="15450"/>
   </bookViews>
   <sheets>
     <sheet name="summary_mean_totals" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,24 +409,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -590,70 +572,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="22" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="35" borderId="0" xfId="19" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="33" borderId="0" xfId="19" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="35" borderId="0" xfId="19" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="33" borderId="0" xfId="19" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="35" borderId="0" xfId="19" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="33" borderId="0" xfId="19" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="34" borderId="0" xfId="19" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="34" borderId="0" xfId="19" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="26" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="13" borderId="0" xfId="22" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="13" borderId="0" xfId="22" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="13" borderId="0" xfId="22" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="22" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -702,37 +633,39 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -748,19 +681,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Accent2" dataCellStyle="20% - Accent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G16"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16">
-    <sortCondition ref="A1:A16"/>
+    <sortCondition ref="B1:B16"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="2" name="summary" dataDxfId="6" dataCellStyle="Accent3"/>
-    <tableColumn id="3" name="Trip ID" dataDxfId="5" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="4" name="precipIntensity" dataDxfId="4" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="5" name="precipProbability" dataDxfId="3" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="6" name="temperature" dataDxfId="2" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="7" name="apparentTemperature" dataDxfId="0" dataCellStyle="20% - Accent1"/>
-    <tableColumn id="8" name="windSpeed" dataDxfId="1" dataCellStyle="20% - Accent1"/>
+    <tableColumn id="2" name="summary" dataDxfId="2"/>
+    <tableColumn id="3" name="Trip ID" dataDxfId="0"/>
+    <tableColumn id="4" name="precipIntensity" dataDxfId="1"/>
+    <tableColumn id="5" name="precipProbability" dataDxfId="6"/>
+    <tableColumn id="6" name="temperature" dataDxfId="5"/>
+    <tableColumn id="7" name="apparentTemperature" dataDxfId="4"/>
+    <tableColumn id="8" name="windSpeed" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1066,390 +999,458 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="14" style="16" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25.5703125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" style="1"/>
+    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="20.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.4740740740740701</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8.7816719576719604E-3</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.55693139329805896</v>
+      </c>
+      <c r="E2" s="3">
+        <v>54.859182363315597</v>
+      </c>
+      <c r="F2" s="3">
+        <v>53.911052557319202</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3.7963202821869402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.25937500000000002</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="E3" s="3">
+        <v>61.354999999999997</v>
+      </c>
+      <c r="F3" s="3">
+        <v>62.024999999999999</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.5714285714285701</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>82.099642857142797</v>
+      </c>
+      <c r="F4" s="3">
+        <v>87.090595238095204</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.9383333333333299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="C5" s="4">
+        <v>9.4139916666666698E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.93694999999999995</v>
+      </c>
+      <c r="E5" s="3">
+        <v>57.916386111111102</v>
+      </c>
+      <c r="F5" s="3">
+        <v>57.419680555555502</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3.81826666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.6666666666666601</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.1966666666666599E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.59666666666666601</v>
+      </c>
+      <c r="E6" s="3">
+        <v>33.868333333333297</v>
+      </c>
+      <c r="F6" s="3">
+        <v>28.8816666666666</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6.2091666666666603</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.6666666666666601</v>
+      </c>
+      <c r="C7" s="4">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>7.6666666666666605E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>77.043333333333294</v>
+      </c>
+      <c r="F7" s="3">
+        <v>79.204999999999998</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.6183333333333301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.71428571428571</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.64642857142857E-3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.41892857142857098</v>
+      </c>
+      <c r="E8" s="3">
+        <v>32.431785714285702</v>
+      </c>
+      <c r="F8" s="3">
+        <v>28.9871428571428</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.5032142857142796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.8260869565217299</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.7609739130434699E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.81054161490683196</v>
+      </c>
+      <c r="E9" s="3">
+        <v>53.8329378881987</v>
+      </c>
+      <c r="F9" s="3">
+        <v>52.800018633540297</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4.2002523809523797</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4">
+        <v>8.7499999999999999E-5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.125E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>80.5124776785714</v>
+      </c>
+      <c r="F10" s="3">
+        <v>85.251808035714205</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.7098660714285701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.07751937984496</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.5260243632336601E-5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.0413990402362498E-3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>52.6261347975882</v>
+      </c>
+      <c r="F11" s="3">
+        <v>51.444129125138403</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3.3068740679217399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.0858995137763299</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.08509557253479E-4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.2264438784698E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>50.741817916956002</v>
+      </c>
+      <c r="F12" s="3">
+        <v>49.270543766561197</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3.9148039991253101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2.1688311688311601</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.2476190476190401E-4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2.9229437229437199E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>38.642200216450199</v>
+      </c>
+      <c r="F13" s="3">
+        <v>36.1265967841682</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3.39687724180581</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2.6381461675579301</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.5978984523102099E-4</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3.2576910562204603E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>42.9076530173134</v>
+      </c>
+      <c r="F14" s="3">
+        <v>40.449536831904403</v>
+      </c>
+      <c r="G14" s="2">
+        <v>4.3379864226682399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6">
-        <v>1.9352014010507801</v>
-      </c>
-      <c r="C2" s="12">
-        <v>1.6454007172045701E-5</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2.2671170044199799E-3</v>
-      </c>
-      <c r="E2" s="11">
-        <v>47.0093979442915</v>
-      </c>
-      <c r="F2" s="11">
-        <v>45.539358915019598</v>
-      </c>
-      <c r="G2" s="8">
-        <v>2.83292198315403</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1.27173913043478</v>
-      </c>
-      <c r="C3" s="3">
-        <v>8.4319746376811597E-3</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.56086956521739095</v>
-      </c>
-      <c r="E3" s="10">
-        <v>54.042364130434699</v>
-      </c>
-      <c r="F3" s="10">
-        <v>53.140326086956499</v>
-      </c>
-      <c r="G3" s="7">
-        <v>3.5057518115941999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="14">
-        <v>1.4</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3.47333333333333E-3</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.42399999999999899</v>
-      </c>
-      <c r="E4" s="11">
-        <v>33.241333333333301</v>
-      </c>
-      <c r="F4" s="11">
-        <v>28.9946666666666</v>
-      </c>
-      <c r="G4" s="6">
-        <v>5.8233333333333297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1.71428571428571</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1.1122448979591799E-4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2.3503401360544199E-2</v>
-      </c>
-      <c r="E5" s="11">
-        <v>37.8901462585033</v>
-      </c>
-      <c r="F5" s="11">
-        <v>35.039931972789098</v>
-      </c>
-      <c r="G5" s="7">
-        <v>3.6626394557823101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.27555000000000002</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.97</v>
-      </c>
-      <c r="E6" s="10">
-        <v>50.63</v>
-      </c>
-      <c r="F6" s="10">
-        <v>50.63</v>
-      </c>
-      <c r="G6" s="8">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="B15" s="2">
+        <v>2.7285513361462699</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.38326300984528E-5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2.0196905766526E-3</v>
+      </c>
+      <c r="E15" s="3">
+        <v>47.423988319502001</v>
+      </c>
+      <c r="F15" s="3">
+        <v>46.040928815480399</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.8142822300765298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6">
-        <v>2.0909090909090899</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B16" s="2">
+        <v>2.7857142857142798</v>
+      </c>
+      <c r="C16" s="4">
         <v>0</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D16" s="4">
         <v>0</v>
       </c>
-      <c r="E7" s="9">
-        <v>82.075787878787807</v>
-      </c>
-      <c r="F7" s="9">
-        <v>86.825666666666606</v>
-      </c>
-      <c r="G7" s="7">
-        <v>2.9187424242424198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1.8333333333333299</v>
-      </c>
-      <c r="C8" s="12">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="9">
-        <v>81.650208333333296</v>
-      </c>
-      <c r="F8" s="9">
-        <v>87.090694444444395</v>
-      </c>
-      <c r="G8" s="8">
-        <v>2.5317361111111101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>4.4999999999999999E-4</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E9" s="9">
-        <v>78.237499999999997</v>
-      </c>
-      <c r="F9" s="9">
-        <v>80.664999999999907</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1.3525</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="14">
-        <v>1.375</v>
-      </c>
-      <c r="C10" s="12">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9">
-        <v>80.855625000000003</v>
-      </c>
-      <c r="F10" s="9">
-        <v>85.69</v>
-      </c>
-      <c r="G10" s="8">
-        <v>2.6225000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="7">
-        <v>1.44705882352941</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2.7448549019607801E-2</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.81072941176470503</v>
-      </c>
-      <c r="E11" s="10">
-        <v>53.201768627450903</v>
-      </c>
-      <c r="F11" s="10">
-        <v>52.0374352941176</v>
-      </c>
-      <c r="G11" s="6">
-        <v>4.2145137254901899</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="14">
-        <v>1.3333333333333299</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1.13666666666666E-2</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.59333333333333305</v>
-      </c>
-      <c r="E12" s="11">
-        <v>33.984166666666603</v>
-      </c>
-      <c r="F12" s="11">
-        <v>28.578333333333301</v>
-      </c>
-      <c r="G12" s="6">
-        <v>6.9241666666666601</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="7">
-        <v>1.6278538812785299</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1.16948249619482E-4</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.25007610350076E-2</v>
-      </c>
-      <c r="E13" s="10">
-        <v>51.046590943683398</v>
-      </c>
-      <c r="F13" s="10">
-        <v>49.602350456620997</v>
-      </c>
-      <c r="G13" s="6">
-        <v>3.9180041856925398</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="6">
-        <v>1.8218262806236001</v>
-      </c>
-      <c r="C14" s="4">
-        <v>2.9867748435677101E-4</v>
-      </c>
-      <c r="D14" s="4">
-        <v>3.8342295047194802E-2</v>
-      </c>
-      <c r="E14" s="11">
-        <v>42.429643228338001</v>
-      </c>
-      <c r="F14" s="11">
-        <v>39.7777097783434</v>
-      </c>
-      <c r="G14" s="6">
-        <v>4.5277049528051698</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="7">
-        <v>1.5791666666666599</v>
-      </c>
-      <c r="C15" s="12">
-        <v>2.0295138888888801E-5</v>
-      </c>
-      <c r="D15" s="5">
-        <v>2.5605158730158699E-3</v>
-      </c>
-      <c r="E15" s="10">
-        <v>52.735624652777801</v>
-      </c>
-      <c r="F15" s="10">
-        <v>51.502842311507898</v>
-      </c>
-      <c r="G15" s="7">
-        <v>3.3651915674603101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="14">
-        <v>1.29729729729729</v>
-      </c>
-      <c r="C16" s="3">
-        <v>9.63252252252252E-2</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.94337837837837801</v>
-      </c>
-      <c r="E16" s="9">
-        <v>57.2383783783783</v>
-      </c>
-      <c r="F16" s="9">
-        <v>56.622387387387299</v>
-      </c>
-      <c r="G16" s="7">
-        <v>3.8007657657657599</v>
+      <c r="E16" s="3">
+        <v>80.985068027210801</v>
+      </c>
+      <c r="F16" s="3">
+        <v>84.994693877551001</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.7155442176870701</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>